<commit_message>
Moins bourrin, ajout du tableau, conso RTC
</commit_message>
<xml_diff>
--- a/MATLAB/specModules.xlsx
+++ b/MATLAB/specModules.xlsx
@@ -66,7 +66,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,13 +74,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -92,15 +104,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="11" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Satisfaisant" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -415,7 +431,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,13 +455,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>1.7000000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1">
-        <v>3.6000000000000001E-5</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -453,26 +469,26 @@
         <v>5</v>
       </c>
       <c r="B3" s="1">
-        <v>1.7000000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="C3" s="1">
-        <v>3.6000000000000001E-5</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="C4" s="1">
-        <v>3.6000000000000001E-5</v>
-      </c>
-      <c r="D4">
+      <c r="B4" s="3">
+        <v>1.5E-3</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
         <v>5</v>
       </c>
     </row>
@@ -481,13 +497,13 @@
         <v>7</v>
       </c>
       <c r="B5" s="1">
-        <v>1.7000000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="C5" s="1">
-        <v>3.6000000000000001E-5</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -495,13 +511,13 @@
         <v>8</v>
       </c>
       <c r="B6" s="1">
-        <v>1.7000000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="C6" s="1">
-        <v>3.6000000000000001E-5</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -509,13 +525,13 @@
         <v>9</v>
       </c>
       <c r="B7" s="1">
-        <v>1.7000000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="C7" s="1">
-        <v>3.6000000000000001E-5</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -523,13 +539,13 @@
         <v>10</v>
       </c>
       <c r="B8" s="1">
-        <v>1.7000000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="C8" s="1">
-        <v>3.6000000000000001E-5</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -537,13 +553,13 @@
         <v>11</v>
       </c>
       <c r="B9" s="1">
-        <v>1.7000000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="C9" s="1">
-        <v>3.6000000000000001E-5</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
import par doc excel
</commit_message>
<xml_diff>
--- a/MATLAB/specModules.xlsx
+++ b/MATLAB/specModules.xlsx
@@ -108,9 +108,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="11" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
@@ -431,7 +430,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,116 +449,116 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="B2" s="2">
+        <v>5.5E-2</v>
+      </c>
+      <c r="C2" s="2">
+        <v>3.6000000000000002E-4</v>
+      </c>
+      <c r="D2" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>1.5E-3</v>
       </c>
-      <c r="C4" s="3">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>0.04</v>
       </c>
-      <c r="C5" s="3">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2">
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
         <v>3.3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>1.5E-3</v>
       </c>
-      <c r="C6" s="3">
-        <v>0</v>
-      </c>
-      <c r="D6" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="C7" s="3">
-        <v>0</v>
-      </c>
-      <c r="D7" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="1">
-        <v>0</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B8" s="2">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="1">
-        <v>0</v>
-      </c>
-      <c r="C9" s="1">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
+      <c r="B9" s="2">
+        <v>1.5E-3</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ajout tOn et tOff
</commit_message>
<xml_diff>
--- a/MATLAB/specModules.xlsx
+++ b/MATLAB/specModules.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>nom</t>
   </si>
@@ -60,12 +60,27 @@
   </si>
   <si>
     <t>HX711</t>
+  </si>
+  <si>
+    <t>tOn</t>
+  </si>
+  <si>
+    <t>tOff</t>
+  </si>
+  <si>
+    <t>rOn</t>
+  </si>
+  <si>
+    <t>rOff</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="178" formatCode="0.00000000000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -108,10 +123,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="11" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,15 +443,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -446,120 +468,248 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="3">
         <v>5.5E-2</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="3">
         <v>3.6000000000000002E-4</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="3">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3">
+        <v>60</v>
+      </c>
+      <c r="F2" s="3">
+        <f>D2/(E2+D2)</f>
+        <v>3.2258064516129031E-2</v>
+      </c>
+      <c r="G2" s="3">
+        <f>E2/(E2+D2)</f>
+        <v>0.967741935483871</v>
+      </c>
+      <c r="H2" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="3">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="3">
         <v>0</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="3">
+        <v>2</v>
+      </c>
+      <c r="E3" s="3">
+        <v>60</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" ref="F3:F9" si="0">D3/(E3+D3)</f>
+        <v>3.2258064516129031E-2</v>
+      </c>
+      <c r="G3" s="3">
+        <f t="shared" ref="G3:G9" si="1">E3/(E3+D3)</f>
+        <v>0.967741935483871</v>
+      </c>
+      <c r="H3" s="3">
         <v>3.3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="3">
         <v>1.5E-3</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="3">
         <v>0</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="3">
+        <v>2</v>
+      </c>
+      <c r="E4" s="3">
+        <v>60</v>
+      </c>
+      <c r="F4" s="3">
+        <f t="shared" si="0"/>
+        <v>3.2258064516129031E-2</v>
+      </c>
+      <c r="G4" s="3">
+        <f t="shared" si="1"/>
+        <v>0.967741935483871</v>
+      </c>
+      <c r="H4" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="3">
         <v>0.04</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="3">
         <v>0</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="3">
+        <v>2</v>
+      </c>
+      <c r="E5" s="3">
+        <v>60</v>
+      </c>
+      <c r="F5" s="3">
+        <f t="shared" si="0"/>
+        <v>3.2258064516129031E-2</v>
+      </c>
+      <c r="G5" s="3">
+        <f t="shared" si="1"/>
+        <v>0.967741935483871</v>
+      </c>
+      <c r="H5" s="3">
         <v>3.3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="3">
         <v>1.5E-3</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="3">
         <v>0</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="3">
+        <v>2</v>
+      </c>
+      <c r="E6" s="3">
+        <v>60</v>
+      </c>
+      <c r="F6" s="3">
+        <f t="shared" si="0"/>
+        <v>3.2258064516129031E-2</v>
+      </c>
+      <c r="G6" s="3">
+        <f t="shared" si="1"/>
+        <v>0.967741935483871</v>
+      </c>
+      <c r="H6" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="3">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="3">
         <v>0</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="3">
+        <v>2</v>
+      </c>
+      <c r="E7" s="3">
+        <v>60</v>
+      </c>
+      <c r="F7" s="3">
+        <f t="shared" si="0"/>
+        <v>3.2258064516129031E-2</v>
+      </c>
+      <c r="G7" s="3">
+        <f t="shared" si="1"/>
+        <v>0.967741935483871</v>
+      </c>
+      <c r="H7" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="3">
         <v>0.16400000000000001</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="3">
         <v>0</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="3">
+        <v>30</v>
+      </c>
+      <c r="E8" s="3">
+        <f>24*60*60</f>
+        <v>86400</v>
+      </c>
+      <c r="F8" s="3">
+        <f t="shared" si="0"/>
+        <v>3.4710170079833391E-4</v>
+      </c>
+      <c r="G8" s="3">
+        <f t="shared" si="1"/>
+        <v>0.99965289829920168</v>
+      </c>
+      <c r="H8" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="3">
         <v>1.5E-3</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="3">
         <v>0</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="3">
+        <v>2</v>
+      </c>
+      <c r="E9" s="3">
+        <v>60</v>
+      </c>
+      <c r="F9" s="3">
+        <f t="shared" si="0"/>
+        <v>3.2258064516129031E-2</v>
+      </c>
+      <c r="G9" s="3">
+        <f t="shared" si="1"/>
+        <v>0.967741935483871</v>
+      </c>
+      <c r="H9" s="3">
         <v>5</v>
       </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G13" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>